<commit_message>
updated: working buttons with sched
workign na yung 2 buttons copy paste ko na bukas together with complete buttons and schedules
</commit_message>
<xml_diff>
--- a/assets/Schedules/stiSched.xlsx
+++ b/assets/Schedules/stiSched.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FILES\COLLEGE\Thesis Code\STI ONN\assets\Schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{926097B9-43D6-4363-A8B4-B3B90131BA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C13D29-DD0A-4AD8-A049-81BCE19382B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55863BE4-401B-4882-B69A-C4E923D00DFC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{55863BE4-401B-4882-B69A-C4E923D00DFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Room 301" sheetId="1" r:id="rId1"/>
+    <sheet name="Room 302" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="94">
   <si>
     <t>Time</t>
   </si>
@@ -330,12 +331,166 @@
 LUCENA
 RM301</t>
   </si>
+  <si>
+    <t>NETWORK1 - LEC
+BSIT 402
+ORUGA</t>
+  </si>
+  <si>
+    <t>KEB - LEC 
+BSHM 204
+PINE</t>
+  </si>
+  <si>
+    <t>STRATMAN 
+BSHM 602
+BSBA 602
+BOBIS</t>
+  </si>
+  <si>
+    <t>PQTOOLS - LEC
+BSBA 202
+BOBIS</t>
+  </si>
+  <si>
+    <t>SAM - LEC 
+BSIT 204
+ORUGA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACT RESEARCH - LEC
+BSA 601
+LUCIDO </t>
+  </si>
+  <si>
+    <t>KEB - LEC 
+BSHM 201
+LAMIS</t>
+  </si>
+  <si>
+    <t>SAM - LEC 
+BSIT 201
+ORUGA</t>
+  </si>
+  <si>
+    <t>POP - LEC 
+BSTM 601
+ATIENZA</t>
+  </si>
+  <si>
+    <t>GAMEPROG - LEC
+BSCS 601
+DALUDADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPPP - LEC 
+BSTM 401
+BUSALPA
+</t>
+  </si>
+  <si>
+    <t>BANCATT - LEC 
+HRS 401
+CABRERA</t>
+  </si>
+  <si>
+    <t>MMA FELEC2 
+ADVWEBDESIGN - LEC
+BMMA 601
+DALUDADO</t>
+  </si>
+  <si>
+    <t>SAM - LEC 
+BSIT 202
+ORUGA</t>
+  </si>
+  <si>
+    <t>COPRO 2 - LEC 
+BSIT 201
+CABAHUG</t>
+  </si>
+  <si>
+    <t>SAM - LEC 
+BSIT 203
+ORUGA</t>
+  </si>
+  <si>
+    <t>EPDESIGN - LEC 
+BMMA 201
+REMOQUILLO</t>
+  </si>
+  <si>
+    <t>ETHICS 
+BSIT 201
+QUIZANA</t>
+  </si>
+  <si>
+    <t>WESCUIS - LEC 
+HRS 401
+CABRERA</t>
+  </si>
+  <si>
+    <t>NETWORK1 - LEC
+BSIT 401
+ORUGA</t>
+  </si>
+  <si>
+    <t>KEB - LEC 
+BSHM 203
+PINE</t>
+  </si>
+  <si>
+    <t>KEB - LEC 
+BSHM 202
+LAMIS</t>
+  </si>
+  <si>
+    <t>TM OJT 
+BSTM 801
+PINE</t>
+  </si>
+  <si>
+    <t>COPRO2 - LEC 
+BSIT 202 
+CABAHUG</t>
+  </si>
+  <si>
+    <t>HM OJT 
+BSHM 801
+MALTO</t>
+  </si>
+  <si>
+    <t>INTEPROG - LAB
+BSIT 401
+PALMONES</t>
+  </si>
+  <si>
+    <t>INFOMAGT - LEC
+BSIT 402
+PALMONES</t>
+  </si>
+  <si>
+    <t>ETHICS 
+BSCS 401
+BSBA 202
+ATIENZA</t>
+  </si>
+  <si>
+    <t>FILPROD - LEC 
+BMMA 601
+REMOQUILLO</t>
+  </si>
+  <si>
+    <t>EPDESIGN - LEC 
+BMMA 202
+REMOQUILLO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,8 +505,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +530,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -398,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -415,6 +583,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0121FDB9-FB33-4371-A2EE-408B66A5C16D}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,4 +1458,537 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736D60E9-7251-4C66-819B-578F08BB8B75}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>